<commit_message>
Final layout of board
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KjB22\Desktop\Kicad Projects\BlueSTM32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KjB22\Desktop\Kicad Projects\ENGT481\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7FB91D-50E2-4BCE-87BB-6E66E61DFD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59B8924-4128-4390-9DCE-04405076FC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{EC1EF8A6-F3C8-49CE-B7CB-3A00316C7F8D}"/>
   </bookViews>
@@ -291,10 +291,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B740131C-1951-4028-9296-12DC66D8C51C}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,10 +678,10 @@
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -690,10 +690,10 @@
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -955,7 +955,7 @@
       <c r="C40" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>